<commit_message>
Added Port for positiontracking
</commit_message>
<xml_diff>
--- a/documentation/port mapping.xlsx
+++ b/documentation/port mapping.xlsx
@@ -5,27 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Clemens\Schule\_DA\_github_repo\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\Desktop\camera_controlled_swarm_robots\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6100E5-0EFD-4AEB-9047-B6C2ECED623F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692C74F9-5E1C-4714-B740-5C7962AB3E70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="1275" windowWidth="21600" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>port number</t>
   </si>
@@ -40,6 +49,12 @@
   </si>
   <si>
     <t>server for path generation</t>
+  </si>
+  <si>
+    <t>positiontracking</t>
+  </si>
+  <si>
+    <t>server for positions</t>
   </si>
 </sst>
 </file>
@@ -211,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -492,10 +507,10 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="9" customWidth="1"/>
@@ -529,10 +544,16 @@
         <f>A2+1</f>
         <v>10001</v>
       </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A16" si="0">A3+1</f>
+        <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>10002</v>
       </c>
     </row>

</xml_diff>